<commit_message>
Fixed Accreditation issues, fixed Liscensure issues, started fix on proper naming scheme for Program Name
</commit_message>
<xml_diff>
--- a/test_files/va_24_25.xlsx
+++ b/test_files/va_24_25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andyburnett/Library/Mobile Documents/com~apple~CloudDocs/Desktop/X03.27.25/OVS/Special Projects/catalog/Catelog_v4/24_25_Catalog/modules/frontend/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE299470-ACED-0747-9FA5-CBD7179A2739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C00277-D8EE-D846-9930-3DCCCEB64607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45020" yWindow="540" windowWidth="23600" windowHeight="26760" xr2:uid="{A783529E-05AA-C143-89E1-F41211381BEA}"/>
   </bookViews>
@@ -7308,8 +7308,8 @@
   <dimension ref="A1:V763"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="165" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <pane ySplit="3" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>